<commit_message>
v1.9.13 modified some files
</commit_message>
<xml_diff>
--- a/Список проживающих.xlsx
+++ b/Список проживающих.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAVETTI\PycharmProjects\pythonProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\PycharmProjects\Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E23CA6-2587-483F-987E-B4FF5414829E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="7640"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="242">
   <si>
     <t>Лупенко Никита Александрович</t>
   </si>
@@ -380,389 +372,392 @@
     <t>Марфина Софья Владимировна</t>
   </si>
   <si>
+    <t>Кудрявцева Екатерина Юрьевна</t>
+  </si>
+  <si>
+    <t>Зубреев Антон Игоревич</t>
+  </si>
+  <si>
+    <t>Денисова Виктория Михайловна</t>
+  </si>
+  <si>
+    <t>Леутина Таисия Александровна</t>
+  </si>
+  <si>
+    <t>Зиннурова Дарья Ильдаровна</t>
+  </si>
+  <si>
+    <t>Спынаки Анна Сергеевна</t>
+  </si>
+  <si>
+    <t>Сасина Анастасия Евгеньевна</t>
+  </si>
+  <si>
+    <t>Шипова Татьяна Евгеньевна</t>
+  </si>
+  <si>
+    <t>Стародубенко Лия Алексеевна</t>
+  </si>
+  <si>
+    <t>Титова Екатерина Сергеевна</t>
+  </si>
+  <si>
+    <t>Шамсутдинова Регина Наильевна</t>
+  </si>
+  <si>
+    <t>Блинков Денис Евгеньевич</t>
+  </si>
+  <si>
+    <t>Рыскин Олег Александрович</t>
+  </si>
+  <si>
+    <t>Чанглян Давид Николаевич</t>
+  </si>
+  <si>
+    <t>Абрамов Александр Андреевич</t>
+  </si>
+  <si>
+    <t>Плотников Алексей Евгеньевич</t>
+  </si>
+  <si>
+    <t>Хамицаев Астан Русланович</t>
+  </si>
+  <si>
+    <t>Выборнов Сергей Сергеевич</t>
+  </si>
+  <si>
+    <t>Потапенко Сергей Александрович</t>
+  </si>
+  <si>
+    <t>Беляев Егор Алексеевич</t>
+  </si>
+  <si>
+    <t>Данилин Никита Вячеславович</t>
+  </si>
+  <si>
+    <t>Колесников Алексей Владимирович</t>
+  </si>
+  <si>
+    <t>Селивёрстов Никита Александрович</t>
+  </si>
+  <si>
+    <t>Юпенков Роман Владимирович</t>
+  </si>
+  <si>
+    <t>Пех Данила Сергеевич</t>
+  </si>
+  <si>
+    <t>Тушин Дмитрий Валерьевич</t>
+  </si>
+  <si>
+    <t>Шестов Владислав Алексеевич</t>
+  </si>
+  <si>
+    <t>Мишин Андрей Сергеевич</t>
+  </si>
+  <si>
+    <t>Родионов Владислав Андреевич</t>
+  </si>
+  <si>
+    <t>Рожков Игорь Алексеевич</t>
+  </si>
+  <si>
+    <t>Холхунов Сергей Иванович</t>
+  </si>
+  <si>
+    <t>Косолапова Валерия Александровна</t>
+  </si>
+  <si>
+    <t>Филатова Екатерина Сергеевна</t>
+  </si>
+  <si>
+    <t>Смирнова Ирина Геннадьевна</t>
+  </si>
+  <si>
+    <t>Чепелева Дарья Сергеевна</t>
+  </si>
+  <si>
+    <t>Чуркин Иван Витальевич</t>
+  </si>
+  <si>
+    <t>Чуркин Даниил Витальевич</t>
+  </si>
+  <si>
+    <t>Ибряева Арина Андреевна</t>
+  </si>
+  <si>
+    <t>Косых Анна Васильевна</t>
+  </si>
+  <si>
+    <t>Карнаков Валентин Андреевич</t>
+  </si>
+  <si>
+    <t>Мамедов Алиаскер Эльманович</t>
+  </si>
+  <si>
+    <t>Борох Валентина Николаевна</t>
+  </si>
+  <si>
+    <t>Даушева Алина Фаритовна</t>
+  </si>
+  <si>
+    <t>Солодкова Ольга Викторовна</t>
+  </si>
+  <si>
+    <t>Барабанова Ксения Александровна</t>
+  </si>
+  <si>
+    <t>Михайлова Елизавета Юрьевна</t>
+  </si>
+  <si>
+    <t>Донецкая Ангелина Алексеевна</t>
+  </si>
+  <si>
+    <t>Коврижко Алина Сергеевна</t>
+  </si>
+  <si>
+    <t>Муравьёва Екатерина Андреевна</t>
+  </si>
+  <si>
+    <t>Сычёва Владислава Дмитриевна</t>
+  </si>
+  <si>
+    <t>Гордеева Наталья Александровна</t>
+  </si>
+  <si>
+    <t>Данилова Клавдия Васильевна</t>
+  </si>
+  <si>
+    <t>Шаборкина Ксения Алексеевна</t>
+  </si>
+  <si>
+    <t>Башкатова Дарья Александровна</t>
+  </si>
+  <si>
+    <t>Захаренко Анастасия Кирилловна</t>
+  </si>
+  <si>
+    <t>Войтик Ксения Дмитриевна</t>
+  </si>
+  <si>
+    <t>Орличеня Вербина Васильевна</t>
+  </si>
+  <si>
+    <t>Наземутдинова Валерия Рустемовна</t>
+  </si>
+  <si>
+    <t>Санникова Мария Юрьевна</t>
+  </si>
+  <si>
+    <t>Тараруева Мария Александровна</t>
+  </si>
+  <si>
+    <t>Лебедева Анна Игоревна</t>
+  </si>
+  <si>
+    <t>Матвеева Кристина Васильевна</t>
+  </si>
+  <si>
+    <t>Сидорычева Анна Валерьевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сметанкина Мария Николаевна </t>
+  </si>
+  <si>
+    <t>Тарасова Александра Владимировна</t>
+  </si>
+  <si>
+    <t>Исаева Анна Александровна</t>
+  </si>
+  <si>
+    <t>Тарасова Дарья Антоновна</t>
+  </si>
+  <si>
+    <t>Хохлова Анастасия Максимовна</t>
+  </si>
+  <si>
+    <t>Панкова Софья Денисовна</t>
+  </si>
+  <si>
+    <t>Стрелова Елена Сергеевна</t>
+  </si>
+  <si>
+    <t>Маликова Виктория Александровна</t>
+  </si>
+  <si>
+    <t>Юсупова Дина Венеровна</t>
+  </si>
+  <si>
+    <t>Куменко Ольга Евгеньевна</t>
+  </si>
+  <si>
+    <t>Межова Милана Павловна</t>
+  </si>
+  <si>
+    <t>Татуйко Анастасия Александровна</t>
+  </si>
+  <si>
+    <t>Чурляева Валерия Олеговна</t>
+  </si>
+  <si>
+    <t>Романенко Арина Романовна</t>
+  </si>
+  <si>
+    <t>Третьяк Ирина Андреевна</t>
+  </si>
+  <si>
+    <t>Алиева Патимат Джебраиловна</t>
+  </si>
+  <si>
+    <t>Китаева Елизавета Андреевна</t>
+  </si>
+  <si>
+    <t>Лукьянчикова Ульяна Алексеевна</t>
+  </si>
+  <si>
+    <t>Берешполова Юлия Дмитриевна</t>
+  </si>
+  <si>
+    <t>Серова Виктория Михайловна</t>
+  </si>
+  <si>
+    <t>Шайхутдинова Ирина Дамировна</t>
+  </si>
+  <si>
+    <t>Лебедева Елена Алексеевна</t>
+  </si>
+  <si>
+    <t>Прошакова Мария Андреевна</t>
+  </si>
+  <si>
+    <t>Юдина Ольга Вячеславовна</t>
+  </si>
+  <si>
+    <t>Алексахина Виктория Валерьевна</t>
+  </si>
+  <si>
+    <t>Матюхина Юлия Алексеевна</t>
+  </si>
+  <si>
+    <t>Семина Валерия Олеговна</t>
+  </si>
+  <si>
+    <t>Павлова Ирина Владимировна</t>
+  </si>
+  <si>
+    <t>Терина Мария Денисовна</t>
+  </si>
+  <si>
+    <t>Миннивалиева Гульсина Ирековна</t>
+  </si>
+  <si>
+    <t>Пугачёва Елизавета Сергеевна</t>
+  </si>
+  <si>
+    <t>Соболева Татьяна Юрьевна</t>
+  </si>
+  <si>
+    <t>Белавина Анастасия Алексеевна</t>
+  </si>
+  <si>
+    <t>Кильпиляйнен Арина Николаевна</t>
+  </si>
+  <si>
+    <t>Глущенко Ирина Александровна</t>
+  </si>
+  <si>
+    <t>Давлетбаева Алина Ринатовна</t>
+  </si>
+  <si>
+    <t>Коннова Анастасия Владимировна</t>
+  </si>
+  <si>
+    <t>Фетисенкова Ксения Алексеевна</t>
+  </si>
+  <si>
+    <t>Лапшина Анастасия Андреевна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Семенюк Олеся Игоревна </t>
+  </si>
+  <si>
+    <t>Турищева Екатерина Евгеньевна</t>
+  </si>
+  <si>
+    <t>Ваганова Полина Александровна</t>
+  </si>
+  <si>
+    <t>Волкова Елена Алексеевна</t>
+  </si>
+  <si>
+    <t>Шмарина Анна Александровна</t>
+  </si>
+  <si>
+    <t>Ахрамеева Екатерина Дмитриевна</t>
+  </si>
+  <si>
+    <t>Енгалычева Мария Игоревна</t>
+  </si>
+  <si>
+    <t>Кандыба Анастасия Леонидовна</t>
+  </si>
+  <si>
+    <t>Расулева Василя Иршатовна</t>
+  </si>
+  <si>
+    <t>Гайнетдинова Александра Раисовна</t>
+  </si>
+  <si>
+    <t>Коленкова Татьяна Владимировна</t>
+  </si>
+  <si>
+    <t>Горькова Елена Михайловна</t>
+  </si>
+  <si>
+    <t>Кондратьева Татьяна Михайловна</t>
+  </si>
+  <si>
+    <t>Городилова Наталья Александровна</t>
+  </si>
+  <si>
+    <t>Салимова Ксения Сергеевна</t>
+  </si>
+  <si>
+    <t>Кабалина Екатерина Валерьевна</t>
+  </si>
+  <si>
+    <t>Таламанова Елена Сергеевна</t>
+  </si>
+  <si>
+    <t> 96807980</t>
+  </si>
+  <si>
+    <t> 299911265</t>
+  </si>
+  <si>
+    <t> 177340209</t>
+  </si>
+  <si>
+    <t> 352238302</t>
+  </si>
+  <si>
+    <t> 341777092</t>
+  </si>
+  <si>
+    <t> 501199558</t>
+  </si>
+  <si>
     <t>Алексеева Ксения Романовна</t>
   </si>
   <si>
-    <t>Кудрявцева Екатерина Юрьевна</t>
-  </si>
-  <si>
-    <t>Зубреев Антон Игоревич</t>
-  </si>
-  <si>
-    <t>Денисова Виктория Михайловна</t>
-  </si>
-  <si>
-    <t>Леутина Таисия Александровна</t>
-  </si>
-  <si>
-    <t>Зиннурова Дарья Ильдаровна</t>
-  </si>
-  <si>
-    <t>Спынаки Анна Сергеевна</t>
-  </si>
-  <si>
-    <t>Сасина Анастасия Евгеньевна</t>
-  </si>
-  <si>
-    <t>Шипова Татьяна Евгеньевна</t>
-  </si>
-  <si>
-    <t>Стародубенко Лия Алексеевна</t>
-  </si>
-  <si>
-    <t>Титова Екатерина Сергеевна</t>
-  </si>
-  <si>
-    <t>Шамсутдинова Регина Наильевна</t>
-  </si>
-  <si>
-    <t>Блинков Денис Евгеньевич</t>
-  </si>
-  <si>
-    <t>Рыскин Олег Александрович</t>
-  </si>
-  <si>
-    <t>Чанглян Давид Николаевич</t>
-  </si>
-  <si>
-    <t>Абрамов Александр Андреевич</t>
-  </si>
-  <si>
-    <t>Плотников Алексей Евгеньевич</t>
-  </si>
-  <si>
-    <t>Хамицаев Астан Русланович</t>
-  </si>
-  <si>
-    <t>Выборнов Сергей Сергеевич</t>
-  </si>
-  <si>
-    <t>Потапенко Сергей Александрович</t>
-  </si>
-  <si>
-    <t>Беляев Егор Алексеевич</t>
-  </si>
-  <si>
-    <t>Данилин Никита Вячеславович</t>
-  </si>
-  <si>
-    <t>Колесников Алексей Владимирович</t>
-  </si>
-  <si>
-    <t>Селивёрстов Никита Александрович</t>
-  </si>
-  <si>
-    <t>Юпенков Роман Владимирович</t>
-  </si>
-  <si>
-    <t>Пех Данила Сергеевич</t>
-  </si>
-  <si>
-    <t>Тушин Дмитрий Валерьевич</t>
-  </si>
-  <si>
-    <t>Шестов Владислав Алексеевич</t>
-  </si>
-  <si>
-    <t>Мишин Андрей Сергеевич</t>
-  </si>
-  <si>
-    <t>Родионов Владислав Андреевич</t>
-  </si>
-  <si>
-    <t>Рожков Игорь Алексеевич</t>
-  </si>
-  <si>
-    <t>Холхунов Сергей Иванович</t>
-  </si>
-  <si>
-    <t>Косолапова Валерия Александровна</t>
-  </si>
-  <si>
-    <t>Филатова Екатерина Сергеевна</t>
-  </si>
-  <si>
-    <t>Смирнова Ирина Геннадьевна</t>
-  </si>
-  <si>
-    <t>Чепелева Дарья Сергеевна</t>
-  </si>
-  <si>
-    <t>Чуркин Иван Витальевич</t>
-  </si>
-  <si>
-    <t>Чуркин Даниил Витальевич</t>
-  </si>
-  <si>
-    <t>Ибряева Арина Андреевна</t>
-  </si>
-  <si>
-    <t>Косых Анна Васильевна</t>
-  </si>
-  <si>
-    <t>Карнаков Валентин Андреевич</t>
-  </si>
-  <si>
-    <t>Мамедов Алиаскер Эльманович</t>
-  </si>
-  <si>
-    <t>Борох Валентина Николаевна</t>
-  </si>
-  <si>
-    <t>Даушева Алина Фаритовна</t>
-  </si>
-  <si>
-    <t>Солодкова Ольга Викторовна</t>
-  </si>
-  <si>
-    <t>Барабанова Ксения Александровна</t>
-  </si>
-  <si>
-    <t>Михайлова Елизавета Юрьевна</t>
-  </si>
-  <si>
-    <t>Донецкая Ангелина Алексеевна</t>
-  </si>
-  <si>
-    <t>Коврижко Алина Сергеевна</t>
-  </si>
-  <si>
-    <t>Муравьёва Екатерина Андреевна</t>
-  </si>
-  <si>
-    <t>Сычёва Владислава Дмитриевна</t>
-  </si>
-  <si>
-    <t>Гордеева Наталья Александровна</t>
-  </si>
-  <si>
-    <t>Данилова Клавдия Васильевна</t>
-  </si>
-  <si>
-    <t>Шаборкина Ксения Алексеевна</t>
-  </si>
-  <si>
-    <t>Башкатова Дарья Александровна</t>
-  </si>
-  <si>
-    <t>Захаренко Анастасия Кирилловна</t>
-  </si>
-  <si>
-    <t>Войтик Ксения Дмитриевна</t>
-  </si>
-  <si>
-    <t>Орличеня Вербина Васильевна</t>
-  </si>
-  <si>
-    <t>Наземутдинова Валерия Рустемовна</t>
-  </si>
-  <si>
-    <t>Санникова Мария Юрьевна</t>
-  </si>
-  <si>
-    <t>Тараруева Мария Александровна</t>
-  </si>
-  <si>
-    <t>Лебедева Анна Игоревна</t>
-  </si>
-  <si>
-    <t>Матвеева Кристина Васильевна</t>
-  </si>
-  <si>
-    <t>Сидорычева Анна Валерьевна</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сметанкина Мария Николаевна </t>
-  </si>
-  <si>
-    <t>Тарасова Александра Владимировна</t>
-  </si>
-  <si>
-    <t>Исаева Анна Александровна</t>
-  </si>
-  <si>
-    <t>Тарасова Дарья Антоновна</t>
-  </si>
-  <si>
-    <t>Хохлова Анастасия Максимовна</t>
-  </si>
-  <si>
-    <t>Панкова Софья Денисовна</t>
-  </si>
-  <si>
-    <t>Стрелова Елена Сергеевна</t>
-  </si>
-  <si>
-    <t>Маликова Виктория Александровна</t>
-  </si>
-  <si>
-    <t>Юсупова Дина Венеровна</t>
-  </si>
-  <si>
-    <t>Куменко Ольга Евгеньевна</t>
-  </si>
-  <si>
-    <t>Межова Милана Павловна</t>
-  </si>
-  <si>
-    <t>Татуйко Анастасия Александровна</t>
-  </si>
-  <si>
-    <t>Чурляева Валерия Олеговна</t>
-  </si>
-  <si>
-    <t>Романенко Арина Романовна</t>
-  </si>
-  <si>
-    <t>Третьяк Ирина Андреевна</t>
-  </si>
-  <si>
-    <t>Алиева Патимат Джебраиловна</t>
-  </si>
-  <si>
-    <t>Китаева Елизавета Андреевна</t>
-  </si>
-  <si>
-    <t>Лукьянчикова Ульяна Алексеевна</t>
-  </si>
-  <si>
-    <t>Берешполова Юлия Дмитриевна</t>
-  </si>
-  <si>
-    <t>Серова Виктория Михайловна</t>
-  </si>
-  <si>
-    <t>Шайхутдинова Ирина Дамировна</t>
-  </si>
-  <si>
-    <t>Лебедева Елена Алексеевна</t>
-  </si>
-  <si>
-    <t>Прошакова Мария Андреевна</t>
-  </si>
-  <si>
-    <t>Юдина Ольга Вячеславовна</t>
-  </si>
-  <si>
-    <t>Алексахина Виктория Валерьевна</t>
-  </si>
-  <si>
-    <t>Матюхина Юлия Алексеевна</t>
-  </si>
-  <si>
-    <t>Семина Валерия Олеговна</t>
-  </si>
-  <si>
-    <t>Павлова Ирина Владимировна</t>
-  </si>
-  <si>
-    <t>Терина Мария Денисовна</t>
-  </si>
-  <si>
-    <t>Миннивалиева Гульсина Ирековна</t>
-  </si>
-  <si>
-    <t>Пугачёва Елизавета Сергеевна</t>
-  </si>
-  <si>
-    <t>Соболева Татьяна Юрьевна</t>
-  </si>
-  <si>
-    <t>Белавина Анастасия Алексеевна</t>
-  </si>
-  <si>
-    <t>Кильпиляйнен Арина Николаевна</t>
-  </si>
-  <si>
-    <t>Глущенко Ирина Александровна</t>
-  </si>
-  <si>
-    <t>Давлетбаева Алина Ринатовна</t>
-  </si>
-  <si>
-    <t>Коннова Анастасия Владимировна</t>
-  </si>
-  <si>
-    <t>Фетисенкова Ксения Алексеевна</t>
-  </si>
-  <si>
-    <t>Лапшина Анастасия Андреевна</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Семенюк Олеся Игоревна </t>
-  </si>
-  <si>
-    <t>Турищева Екатерина Евгеньевна</t>
-  </si>
-  <si>
-    <t>Ваганова Полина Александровна</t>
-  </si>
-  <si>
-    <t>Волкова Елена Алексеевна</t>
-  </si>
-  <si>
-    <t>Шмарина Анна Александровна</t>
-  </si>
-  <si>
-    <t>Ахрамеева Екатерина Дмитриевна</t>
-  </si>
-  <si>
-    <t>Енгалычева Мария Игоревна</t>
-  </si>
-  <si>
-    <t>Кандыба Анастасия Леонидовна</t>
-  </si>
-  <si>
-    <t>Расулева Василя Иршатовна</t>
-  </si>
-  <si>
-    <t>Гайнетдинова Александра Раисовна</t>
-  </si>
-  <si>
-    <t>Коленкова Татьяна Владимировна</t>
-  </si>
-  <si>
-    <t>Горькова Елена Михайловна</t>
-  </si>
-  <si>
-    <t>Кондратьева Татьяна Михайловна</t>
-  </si>
-  <si>
-    <t>Городилова Наталья Александровна</t>
-  </si>
-  <si>
-    <t>Салимова Ксения Сергеевна</t>
-  </si>
-  <si>
-    <t>Кабалина Екатерина Валерьевна</t>
-  </si>
-  <si>
-    <t>Таламанова Елена Сергеевна</t>
-  </si>
-  <si>
-    <t> 96807980</t>
-  </si>
-  <si>
-    <t> 299911265</t>
-  </si>
-  <si>
-    <t> 177340209</t>
-  </si>
-  <si>
-    <t> 352238302</t>
-  </si>
-  <si>
-    <t> 341777092</t>
-  </si>
-  <si>
-    <t> 501199558</t>
+    <t>Кобелева Татьяна Дмитриевна</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -770,6 +765,21 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="5">
@@ -810,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -818,6 +828,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1131,22 +1143,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C235"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="B235" sqref="B235"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="E241" sqref="E241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.6328125" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1154,7 +1166,7 @@
         <v>243750729</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1162,7 +1174,7 @@
         <v>282218810</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1170,7 +1182,7 @@
         <v>144140626</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1190,7 @@
         <v>66183876</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>390678051</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1194,7 +1206,7 @@
         <v>226096269</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>190977369</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>167173539</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1218,7 +1230,7 @@
         <v>253421603</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>78610654</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>270391646</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>191320361</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1250,7 +1262,7 @@
         <v>194800115</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>224336478</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>200311554</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>172994040</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1282,7 +1294,7 @@
         <v>143562774</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>95087414</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>205005632</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>162182524</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1314,7 +1326,7 @@
         <v>559358664</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1322,7 +1334,7 @@
         <v>540613980</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>108855486</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1338,7 +1350,7 @@
         <v>197398042</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>225377416</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1366,7 @@
         <v>164973911</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>269433090</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>180191576</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>192656101</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1386,12 +1398,12 @@
         <v>119694261</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>211401628</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1407,7 +1419,7 @@
         <v>268428272</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1415,7 +1427,7 @@
         <v>295205789</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1423,7 +1435,7 @@
         <v>327451617</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1431,7 +1443,7 @@
         <v>143361167</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1439,7 +1451,7 @@
         <v>135618794</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1459,7 @@
         <v>113355162</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1455,7 +1467,7 @@
         <v>83778053</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1463,7 +1475,7 @@
         <v>109853420</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1471,7 +1483,7 @@
         <v>150126347</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1479,7 +1491,7 @@
         <v>182185619</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1487,7 +1499,7 @@
         <v>96814361</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1495,7 +1507,7 @@
         <v>156397844</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1503,12 +1515,12 @@
         <v>92731345</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1516,7 +1528,7 @@
         <v>137130543</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1524,7 +1536,7 @@
         <v>504275858</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1532,7 +1544,7 @@
         <v>177752220</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1540,7 +1552,7 @@
         <v>410937534</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1548,7 +1560,7 @@
         <v>137600009</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1556,7 +1568,7 @@
         <v>199853434</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1564,7 +1576,7 @@
         <v>145752566</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>57683251</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -1580,7 +1592,7 @@
         <v>131335311</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -1588,7 +1600,7 @@
         <v>222647814</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -1596,7 +1608,7 @@
         <v>212672786</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1604,7 +1616,7 @@
         <v>186317335</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1612,7 +1624,7 @@
         <v>177968499</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
@@ -1620,7 +1632,7 @@
         <v>180932058</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>156292402</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -1636,7 +1648,7 @@
         <v>183165408</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>196069057</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -1652,12 +1664,12 @@
         <v>176064235</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -1665,7 +1677,7 @@
         <v>185215592</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>219462996</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -1681,7 +1693,7 @@
         <v>503275367</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>209627375</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>146873744</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -1705,7 +1717,7 @@
         <v>157424970</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>71</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>450082917</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -1721,7 +1733,7 @@
         <v>171949230</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -1729,12 +1741,12 @@
         <v>324872980</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1742,12 +1754,12 @@
         <v>250339333</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1755,7 +1767,7 @@
         <v>197950446</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1763,7 +1775,7 @@
         <v>114075926</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1771,7 +1783,7 @@
         <v>124758384</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1779,7 +1791,7 @@
         <v>258009994</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -1787,7 +1799,7 @@
         <v>120195455</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>168321875</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
@@ -1803,7 +1815,7 @@
         <v>141510752</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -1811,7 +1823,7 @@
         <v>100293859</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>85</v>
       </c>
@@ -1819,12 +1831,12 @@
         <v>174603058</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -1832,7 +1844,7 @@
         <v>76170184</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -1840,7 +1852,7 @@
         <v>147224489</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -1848,7 +1860,7 @@
         <v>199518663</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -1856,7 +1868,7 @@
         <v>210855239</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -1864,7 +1876,7 @@
         <v>330640449</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -1872,7 +1884,7 @@
         <v>146396070</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -1880,12 +1892,12 @@
         <v>95492796</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -1893,7 +1905,7 @@
         <v>141267790</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -1901,7 +1913,7 @@
         <v>153634984</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -1909,7 +1921,7 @@
         <v>44861609</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -1917,7 +1929,7 @@
         <v>142229245</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -1925,7 +1937,7 @@
         <v>317815110</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -1933,7 +1945,7 @@
         <v>192620391</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -1941,20 +1953,20 @@
         <v>155763805</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -1962,7 +1974,7 @@
         <v>232184513</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -1970,7 +1982,7 @@
         <v>277790502</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -1978,7 +1990,7 @@
         <v>182494284</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -1986,7 +1998,7 @@
         <v>174926746</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>108</v>
       </c>
@@ -1994,7 +2006,7 @@
         <v>101821792</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>198950390</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2010,7 +2022,7 @@
         <v>169882720</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -2018,12 +2030,12 @@
         <v>118816935</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -2031,7 +2043,7 @@
         <v>442633744</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -2039,943 +2051,956 @@
         <v>157902190</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B116" s="5">
+        <v>192062697</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>115</v>
-      </c>
-      <c r="B116">
-        <v>192062697</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>116</v>
       </c>
       <c r="B117">
         <v>178772592</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>171388030</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119">
         <v>169290021</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>98716288</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" t="s">
-        <v>121</v>
       </c>
       <c r="B122">
         <v>143454798</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>190964122</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>138604228</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>98363149</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>140255360</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>201218764</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>211809712</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>183550586</v>
       </c>
-      <c r="C129">
-        <v>503424983</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" t="s">
-        <v>130</v>
       </c>
       <c r="B131">
         <v>233037678</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>288488294</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>501113658</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>107288138</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>160893193</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>194499929</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>212560945</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>108092672</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>145893810</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>65909221</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>176569515</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>172628438</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>287092244</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>85865097</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>185780136</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>144</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>145</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" t="s">
-        <v>146</v>
       </c>
       <c r="B147">
         <v>147448693</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>220126295</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>147</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>148</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" t="s">
-        <v>149</v>
       </c>
       <c r="B150">
         <v>133913457</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>150</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" t="s">
-        <v>151</v>
       </c>
       <c r="B152">
         <v>260375334</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" t="s">
-        <v>153</v>
       </c>
       <c r="B154">
         <v>105553587</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>102979188</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>118550205</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>175683055</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>296319225</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>171639076</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>359566718</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>229853934</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162">
         <v>53141814</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163">
         <v>162215835</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>162</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>163</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
-        <v>164</v>
       </c>
       <c r="B165">
         <v>233121745</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166">
         <v>151211440</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167">
         <v>195880590</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168">
         <v>159381450</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169">
         <v>155739744</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170">
         <v>258382225</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171">
         <v>245076027</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172">
         <v>118004022</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>165868073</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>109278901</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>241100783</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>146373752</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>82097583</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>178</v>
       </c>
       <c r="B179">
         <v>144897805</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>192260144</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181">
         <v>207826855</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182">
         <v>236807782</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183">
         <v>350326598</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184">
         <v>135710575</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185">
         <v>178625151</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>184</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
         <v>185</v>
-      </c>
-      <c r="B186" s="4" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
-        <v>186</v>
       </c>
       <c r="B187">
         <v>164668351</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188">
         <v>176092335</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189">
         <v>200565730</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190">
         <v>287790099</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191">
         <v>269518853</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192">
         <v>331829115</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193">
         <v>179463737</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194">
         <v>100015387</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>195</v>
       </c>
       <c r="B196">
         <v>110589466</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
+        <v>195</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
         <v>196</v>
-      </c>
-      <c r="B197" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>197</v>
       </c>
       <c r="B198">
         <v>291923835</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>147075291</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>171813394</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201">
         <v>222881820</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202">
         <v>285375497</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203">
         <v>156782713</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204">
         <v>203096660</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205">
         <v>139284988</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206">
         <v>203890253</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207">
         <v>227758653</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208">
         <v>189061694</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209">
         <v>188226676</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210">
         <v>175633875</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211">
         <v>194187303</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212">
         <v>500671692</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213">
         <v>154541686</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214">
         <v>134354944</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215">
         <v>338408421</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216">
         <v>67845167</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217">
         <v>414410038</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218">
         <v>180158123</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219">
         <v>253746479</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220">
         <v>195752295</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221">
         <v>167112083</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222">
         <v>243998586</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223">
         <v>279877713</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224">
         <v>105414207</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225">
         <v>57480772</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226">
         <v>53062512</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227">
         <v>116097400</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228">
         <v>66434500</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
-        <v>229</v>
       </c>
       <c r="B230">
         <v>147913712</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231">
         <v>105841204</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
-        <v>232</v>
       </c>
       <c r="B233">
         <v>184036634</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234">
         <v>119920180</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235">
         <v>140025919</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>241</v>
+      </c>
+      <c r="B236" s="6">
+        <v>343618297</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>127</v>
+      </c>
+      <c r="B237">
+        <v>503424983</v>
       </c>
     </row>
   </sheetData>

</xml_diff>